<commit_message>
adiciona contato ao dicionário de dados
</commit_message>
<xml_diff>
--- a/Banco de Dados/Modelagem de Dados/Dicionário de Dados.xlsx
+++ b/Banco de Dados/Modelagem de Dados/Dicionário de Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moise\Documents\GitHub\YogaCommerce\Banco de Dados\Modelagem de Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D660905B-B683-4C63-818E-41D3B8E8619B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9025A974-522E-4A82-AFBD-A45118C345A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13710" yWindow="615" windowWidth="13815" windowHeight="12885" xr2:uid="{779EC71D-9CF7-46E6-8466-F39F166F623A}"/>
+    <workbookView xWindow="11355" yWindow="0" windowWidth="17550" windowHeight="15585" xr2:uid="{779EC71D-9CF7-46E6-8466-F39F166F623A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="102">
   <si>
     <t>Cliente</t>
   </si>
@@ -318,13 +318,40 @@
   </si>
   <si>
     <t>Nome do produto</t>
+  </si>
+  <si>
+    <t>Contato</t>
+  </si>
+  <si>
+    <t>ID_Contato</t>
+  </si>
+  <si>
+    <t>Telefone_Cliente</t>
+  </si>
+  <si>
+    <t>Email_Cliente</t>
+  </si>
+  <si>
+    <t>Titulo_Problema</t>
+  </si>
+  <si>
+    <t>Descrição_Problema</t>
+  </si>
+  <si>
+    <t>Código de identificação do contato</t>
+  </si>
+  <si>
+    <t>Código de identificação do cliete</t>
+  </si>
+  <si>
+    <t>Titulo do problema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,10 +368,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -364,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -372,6 +408,19 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -417,9 +466,6 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -434,8 +480,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B78AE25A-4EA5-4661-89E4-D13E2835827B}" name="Table2" displayName="Table2" ref="A1:G54" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:G54" xr:uid="{B78AE25A-4EA5-4661-89E4-D13E2835827B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B78AE25A-4EA5-4661-89E4-D13E2835827B}" name="Table2" displayName="Table2" ref="A1:G62" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:G62" xr:uid="{B78AE25A-4EA5-4661-89E4-D13E2835827B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -445,13 +491,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C5177385-19EF-4E5B-9FA3-98D8850B6FBD}" name="Tabela" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{A5627ABD-5E4F-47CA-965F-87AFE093AE3C}" name="Nome da Coluna" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{962ABC5E-79B1-4564-A55B-A167900616C0}" name="Tipo de Dados" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{023890EC-F9EA-4F16-A138-B71338BEACF3}" name="Comprimento" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{1C0457BF-A431-4595-912F-AAC6FA9482C2}" name="Restrições" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1D2B34D4-C790-4588-813C-EE9DBC1E852F}" name="Valor Padrão" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{C7C3E046-3B88-4E61-B662-F122AB0C8172}" name="Descrição" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C5177385-19EF-4E5B-9FA3-98D8850B6FBD}" name="Tabela" totalsRowLabel="Total" dataDxfId="0" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{A5627ABD-5E4F-47CA-965F-87AFE093AE3C}" name="Nome da Coluna" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{962ABC5E-79B1-4564-A55B-A167900616C0}" name="Tipo de Dados" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{023890EC-F9EA-4F16-A138-B71338BEACF3}" name="Comprimento" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{1C0457BF-A431-4595-912F-AAC6FA9482C2}" name="Restrições" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{1D2B34D4-C790-4588-813C-EE9DBC1E852F}" name="Valor Padrão" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{C7C3E046-3B88-4E61-B662-F122AB0C8172}" name="Descrição" totalsRowFunction="count" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -774,28 +820,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D1BC74-CADB-45F2-82B5-D313754B1CA2}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -818,7 +864,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.5">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -841,7 +887,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -862,7 +908,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -883,7 +929,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
@@ -904,7 +950,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -925,7 +971,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -946,7 +992,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -967,7 +1013,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -988,8 +1034,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.5">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1011,7 +1060,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1031,7 +1081,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1051,8 +1102,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="28.5">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1074,7 +1128,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="28.5">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1094,8 +1149,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.5">
-      <c r="A18" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1117,7 +1175,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.5">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1137,7 +1196,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="28.5">
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
@@ -1157,7 +1217,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="28.5">
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1235,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.5">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
@@ -1194,8 +1256,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.5">
-      <c r="A24" s="1" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1217,7 +1282,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.5">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1237,7 +1303,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.5">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1254,7 +1321,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.5">
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1274,8 +1342,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="28.5">
-      <c r="A29" s="1" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1297,7 +1368,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1317,7 +1389,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.5">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
       <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1337,7 +1410,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>21</v>
       </c>
@@ -1357,7 +1431,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1374,7 +1449,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
@@ -1388,7 +1464,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1408,7 +1485,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
       <c r="B36" s="1" t="s">
         <v>25</v>
       </c>
@@ -1428,8 +1506,11 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="28.5">
-      <c r="A38" s="1" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1451,7 +1532,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
@@ -1471,8 +1553,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.5">
-      <c r="A41" s="1" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1494,7 +1579,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.5">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
         <v>1</v>
       </c>
@@ -1514,7 +1600,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.5">
+    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
         <v>34</v>
       </c>
@@ -1534,8 +1621,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.5">
-      <c r="A45" s="1" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -1557,7 +1647,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="28.5">
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
       <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1668,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.5">
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
       <c r="B47" s="1" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1689,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
       <c r="B48" s="1" t="s">
         <v>35</v>
       </c>
@@ -1617,7 +1710,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
       <c r="B49" s="1" t="s">
         <v>36</v>
       </c>
@@ -1634,7 +1728,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
       <c r="B50" s="1" t="s">
         <v>90</v>
       </c>
@@ -1654,8 +1749,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="28.5">
-      <c r="A52" s="1" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1677,7 +1775,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="28.5">
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
       <c r="B53" s="1" t="s">
         <v>34</v>
       </c>
@@ -1697,7 +1796,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
       <c r="B54" s="1" t="s">
         <v>17</v>
       </c>
@@ -1715,6 +1815,155 @@
       </c>
       <c r="G54" s="2" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>